<commit_message>
Two main changes. (1) The therapy.pars object has been deleted. (2) The par_table, apply_summary, and survival_summary functions have been moved to the Shiny app
</commit_message>
<xml_diff>
--- a/data-raw/cost.xlsx
+++ b/data-raw/cost.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340"/>
   </bookViews>
   <sheets>
-    <sheet name="RData" sheetId="9" r:id="rId1"/>
+    <sheet name="Cost" sheetId="9" r:id="rId1"/>
+    <sheet name="Lookup" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
   <si>
     <t>50 mg QW</t>
   </si>
@@ -258,6 +259,48 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>abtivmtx</t>
+  </si>
+  <si>
+    <t>adamtx</t>
+  </si>
+  <si>
+    <t>etnmtx</t>
+  </si>
+  <si>
+    <t>golmtx</t>
+  </si>
+  <si>
+    <t>ifxmtx</t>
+  </si>
+  <si>
+    <t>placebo</t>
+  </si>
+  <si>
+    <t>tczmtx</t>
+  </si>
+  <si>
+    <t>czpmtx</t>
+  </si>
+  <si>
+    <t>abtscmtx</t>
+  </si>
+  <si>
+    <t>nbt</t>
+  </si>
+  <si>
+    <t>rtxmtx</t>
+  </si>
+  <si>
+    <t>tofmtx</t>
+  </si>
+  <si>
+    <t>agent1</t>
+  </si>
+  <si>
+    <t>agent2</t>
   </si>
 </sst>
 </file>
@@ -375,8 +418,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -630,7 +675,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -716,6 +761,7 @@
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -801,6 +847,7 @@
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1082,7 +1129,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1695,4 +1742,226 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(1) Costs are now calculated within sim_iviRA_C, (2) Costs for each therapeutic agent for a treatment are now calculated using iviRA::treat.cost with a new lookup table, (3) discounts and rebates are now sampled in sample_pars asssuming a uniform distribution
</commit_message>
<xml_diff>
--- a/data-raw/cost.xlsx
+++ b/data-raw/cost.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cost" sheetId="9" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
   <si>
     <t>50 mg QW</t>
   </si>
@@ -165,9 +165,6 @@
     <t>ssz</t>
   </si>
   <si>
-    <t>wac_per_unit</t>
-  </si>
-  <si>
     <t>infusion_cost</t>
   </si>
   <si>
@@ -301,6 +298,21 @@
   </si>
   <si>
     <t>agent2</t>
+  </si>
+  <si>
+    <t>price_per_unit</t>
+  </si>
+  <si>
+    <t>loading_dose</t>
+  </si>
+  <si>
+    <t>weight_based</t>
+  </si>
+  <si>
+    <t>discount_lower</t>
+  </si>
+  <si>
+    <t>discount_upper</t>
   </si>
 </sst>
 </file>
@@ -370,7 +382,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -417,8 +429,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -592,8 +613,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -625,27 +656,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -662,11 +672,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -674,8 +682,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -762,6 +815,11 @@
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -848,6 +906,11 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1115,7 +1178,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1123,33 +1186,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5" style="31" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="31" customWidth="1"/>
-    <col min="9" max="9" width="25.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="31" customWidth="1"/>
-    <col min="12" max="13" width="14" style="31" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="31"/>
+    <col min="1" max="1" width="22.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="22" customWidth="1"/>
+    <col min="12" max="12" width="14" style="22" customWidth="1"/>
+    <col min="13" max="14" width="13.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="42" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="28">
+    <row r="1" spans="1:17" s="8" customFormat="1" ht="28">
       <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
@@ -1157,40 +1224,52 @@
         <v>19</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="K1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="42">
+      <c r="P1" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="42">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1210,28 +1289,40 @@
         <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="20">
+        <v>38</v>
+      </c>
+      <c r="H2" s="13">
         <v>26</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="13">
         <v>52</v>
       </c>
-      <c r="J2" s="20">
+      <c r="J2" s="13">
         <v>50</v>
       </c>
-      <c r="K2" s="33" t="s">
-        <v>39</v>
+      <c r="K2" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="L2" s="11">
         <v>1110.5</v>
       </c>
-      <c r="M2" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="42">
+      <c r="M2" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N2" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O2" s="35">
+        <v>0</v>
+      </c>
+      <c r="P2" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="42">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1241,42 +1332,54 @@
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="23">
         <v>40</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="23">
         <v>40</v>
       </c>
-      <c r="G3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="21">
+      <c r="G3" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="14">
         <f>52/4</f>
         <v>13</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="14">
         <f>52/2</f>
         <v>26</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="13">
         <v>40</v>
       </c>
-      <c r="K3" s="33" t="s">
-        <v>39</v>
+      <c r="K3" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="L3" s="11">
         <v>2220.62</v>
       </c>
-      <c r="M3" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="28">
+      <c r="M3" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N3" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O3" s="35">
+        <v>0</v>
+      </c>
+      <c r="P3" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="28">
       <c r="A4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>30</v>
@@ -1285,7 +1388,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="4">
         <v>3</v>
@@ -1294,29 +1397,41 @@
         <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="20">
+        <v>39</v>
+      </c>
+      <c r="H4" s="13">
         <v>5</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="13">
         <f>52/6</f>
         <v>8.6666666666666661</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="13">
         <v>100</v>
       </c>
-      <c r="K4" s="33" t="s">
-        <v>39</v>
+      <c r="K4" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="L4" s="11">
         <v>1113.27</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N4" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O4" s="35">
         <v>164</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="42">
+      <c r="P4" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="42">
       <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
@@ -1336,28 +1451,40 @@
         <v>50</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="20">
+        <v>38</v>
+      </c>
+      <c r="H5" s="13">
         <v>6</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="13">
         <v>12</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="13">
         <v>50</v>
       </c>
-      <c r="K5" s="33" t="s">
-        <v>39</v>
+      <c r="K5" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="L5" s="11">
         <v>3811.18</v>
       </c>
-      <c r="M5" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="42">
+      <c r="M5" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N5" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O5" s="36">
+        <v>0</v>
+      </c>
+      <c r="P5" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="42">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1365,10 +1492,10 @@
         <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="7">
         <v>400</v>
@@ -1377,30 +1504,42 @@
         <v>200</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="22">
+        <v>38</v>
+      </c>
+      <c r="H6" s="15">
         <v>8</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="15">
         <v>26</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="13">
         <v>400</v>
       </c>
-      <c r="K6" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="23">
+      <c r="K6" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="16">
         <v>3679.87</v>
       </c>
-      <c r="M6" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="M6" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N6" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O6" s="37">
+        <v>0</v>
+      </c>
+      <c r="P6" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>32</v>
@@ -1409,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="3">
         <v>750</v>
@@ -1418,7 +1557,7 @@
         <v>750</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="3">
         <v>8</v>
@@ -1427,31 +1566,43 @@
         <f>52/4</f>
         <v>13</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="13">
         <v>250</v>
       </c>
-      <c r="K7" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="24">
+      <c r="K7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="17">
         <v>931.16</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N7" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O7" s="38">
         <v>164</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" s="28" customFormat="1" ht="28">
+      <c r="P7" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="20" customFormat="1" ht="28">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="7">
         <v>125</v>
@@ -1460,7 +1611,7 @@
         <v>125</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="7">
         <v>26</v>
@@ -1471,17 +1622,29 @@
       <c r="J8" s="7">
         <v>125</v>
       </c>
-      <c r="K8" s="33" t="s">
-        <v>39</v>
+      <c r="K8" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="L8" s="12">
         <v>957.14</v>
       </c>
-      <c r="M8" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28">
+      <c r="M8" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N8" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O8" s="35">
+        <v>164</v>
+      </c>
+      <c r="P8" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="28">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1492,7 +1655,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3">
         <v>162</v>
@@ -1501,7 +1664,7 @@
         <v>162</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="3">
         <f>26/2</f>
@@ -1514,17 +1677,29 @@
       <c r="J9" s="3">
         <v>162</v>
       </c>
-      <c r="K9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="25">
+      <c r="K9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="18">
         <v>898.31</v>
       </c>
-      <c r="M9" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="28" customFormat="1">
+      <c r="M9" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N9" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O9" s="39">
+        <v>0</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="20" customFormat="1">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1532,10 +1707,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5">
         <v>1000</v>
@@ -1544,7 +1719,7 @@
         <v>1000</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="3">
         <v>4</v>
@@ -1556,19 +1731,31 @@
       <c r="J10" s="5">
         <v>500</v>
       </c>
-      <c r="K10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="29">
+      <c r="K10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="21">
         <v>4176.1000000000004</v>
       </c>
-      <c r="M10" s="30">
+      <c r="M10" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N10" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O10" s="40">
         <v>164</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="P10" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -1577,7 +1764,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1">
         <v>5</v>
@@ -1586,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1">
         <f>26*7*2</f>
@@ -1599,17 +1786,29 @@
       <c r="J11" s="1">
         <v>5</v>
       </c>
-      <c r="K11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="27">
+      <c r="K11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="19">
         <v>63.26</v>
       </c>
-      <c r="M11" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="M11" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N11" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O11" s="41">
+        <v>0</v>
+      </c>
+      <c r="P11" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1620,7 +1819,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="5">
         <v>15</v>
@@ -1629,7 +1828,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="5">
         <v>26</v>
@@ -1640,17 +1839,29 @@
       <c r="J12" s="1">
         <v>15</v>
       </c>
-      <c r="K12" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="27">
+      <c r="K12" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="19">
         <v>32.418750000000003</v>
       </c>
-      <c r="M12" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="M12" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N12" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O12" s="41">
+        <v>0</v>
+      </c>
+      <c r="P12" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1661,7 +1872,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="5">
         <v>400</v>
@@ -1670,7 +1881,7 @@
         <v>400</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="5">
         <v>182</v>
@@ -1681,17 +1892,29 @@
       <c r="J13" s="1">
         <v>200</v>
       </c>
-      <c r="K13" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="27">
+      <c r="K13" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="19">
         <v>3.18</v>
       </c>
-      <c r="M13" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="M13" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N13" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O13" s="41">
+        <v>0</v>
+      </c>
+      <c r="P13" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1699,10 +1922,10 @@
         <v>35</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="E14" s="5">
         <v>2</v>
@@ -1711,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="5">
         <v>182</v>
@@ -1722,13 +1945,25 @@
       <c r="J14" s="1">
         <v>0.5</v>
       </c>
-      <c r="K14" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="27">
+      <c r="K14" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="19">
         <v>0.47</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="N14" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="O14" s="41">
+        <v>0</v>
+      </c>
+      <c r="P14" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="33">
         <v>0</v>
       </c>
     </row>
@@ -1748,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1759,14 +1994,14 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
@@ -1774,19 +2009,19 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="31" t="s">
-        <v>68</v>
+      <c r="A3" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="31" t="s">
-        <v>69</v>
+      <c r="A4" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -1796,7 +2031,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
@@ -1804,8 +2039,8 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="31" t="s">
-        <v>70</v>
+      <c r="A6" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1815,7 +2050,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
@@ -1823,8 +2058,8 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="31" t="s">
-        <v>71</v>
+      <c r="A8" s="22" t="s">
+        <v>70</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -1834,8 +2069,8 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="31" t="s">
-        <v>72</v>
+      <c r="A9" s="22" t="s">
+        <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -1845,16 +2080,16 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="22" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="31" t="s">
-        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -1864,7 +2099,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
@@ -1872,8 +2107,8 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="31" t="s">
-        <v>75</v>
+      <c r="A13" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -1883,8 +2118,8 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="31" t="s">
-        <v>76</v>
+      <c r="A14" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
@@ -1894,16 +2129,16 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="22" t="s">
         <v>77</v>
-      </c>
-      <c r="B15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="31" t="s">
-        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
@@ -1913,8 +2148,8 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="31" t="s">
-        <v>79</v>
+      <c r="A17" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -1924,7 +2159,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
@@ -1932,7 +2167,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
@@ -1940,7 +2175,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
@@ -1948,7 +2183,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">

</xml_diff>

<commit_message>
Update website with links to user interfaces
</commit_message>
<xml_diff>
--- a/data-raw/cost.xlsx
+++ b/data-raw/cost.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340"/>
   </bookViews>
   <sheets>
     <sheet name="Cost" sheetId="9" r:id="rId1"/>
@@ -1178,7 +1178,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1188,11 +1188,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1498,7 +1498,7 @@
         <v>56</v>
       </c>
       <c r="E6" s="7">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F6" s="7">
         <v>200</v>
@@ -1507,13 +1507,13 @@
         <v>38</v>
       </c>
       <c r="H6" s="15">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I6" s="15">
         <v>26</v>
       </c>
       <c r="J6" s="13">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="K6" s="24" t="s">
         <v>38</v>
@@ -1983,7 +1983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix cost estimates for certolizumab pegol, making dose value 200 mg
</commit_message>
<xml_diff>
--- a/data-raw/cost.xlsx
+++ b/data-raw/cost.xlsx
@@ -1178,7 +1178,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1192,7 +1192,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1519,7 +1519,7 @@
         <v>38</v>
       </c>
       <c r="L6" s="16">
-        <v>3679.87</v>
+        <v>1839.94</v>
       </c>
       <c r="M6" s="43">
         <v>0.2</v>

</xml_diff>

<commit_message>
Correction of costs and AE rate tripe
</commit_message>
<xml_diff>
--- a/data-raw/cost.xlsx
+++ b/data-raw/cost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/GitHub/IVI-RA-v2/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW PROJECTS/IVI/IVI25020 RA CEA update/Model development/IVI-RA-development of v2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA1BA82-3A8A-A24A-B22F-240113C9801E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EBE28E-45D8-5B47-9671-AD43F3200A34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="460" windowWidth="25600" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="119">
   <si>
     <t>50 mg QW</t>
   </si>
@@ -1352,7 +1352,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2583,7 +2583,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2853,9 +2853,11 @@
         <v>90</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">

</xml_diff>

<commit_message>
Correction IFX biosimilar weight based
</commit_message>
<xml_diff>
--- a/data-raw/cost.xlsx
+++ b/data-raw/cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW PROJECTS/IVI/IVI25020 RA CEA update/Model development/IVI-RA-development of v2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EBE28E-45D8-5B47-9671-AD43F3200A34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF44921-A356-204E-8F77-89CA6D1C503B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="460" windowWidth="25600" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="460" windowWidth="25600" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost" sheetId="9" r:id="rId1"/>
@@ -1348,11 +1348,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="11"/>
     </row>
@@ -2582,7 +2582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>

</xml_diff>